<commit_message>
correcciones en impedancia de entrada ej2
</commit_message>
<xml_diff>
--- a/Ej2/Mediciones/tc_tp2_ej2 impedancia de entrada.xlsx
+++ b/Ej2/Mediciones/tc_tp2_ej2 impedancia de entrada.xlsx
@@ -180,23 +180,23 @@
                 <c:pt idx="3">
                   <c:v>20</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="4">
                   <c:v>50</c:v>
                 </c:pt>
+                <c:pt idx="5">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>100</c:v>
+                </c:pt>
                 <c:pt idx="7">
-                  <c:v>70</c:v>
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>500</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>1000</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>500</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>200</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -216,14 +216,23 @@
                 <c:pt idx="3">
                   <c:v>134.44263297095637</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="4">
                   <c:v>125.43197340130185</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="5">
+                  <c:v>121.28166871927192</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>118.6878708752859</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="7">
                   <c:v>118.90067973980632</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>119.58328105304311</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>119.69948197857573</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -651,23 +660,23 @@
                       <c:pt idx="3">
                         <c:v>20</c:v>
                       </c:pt>
+                      <c:pt idx="4">
+                        <c:v>50</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>70</c:v>
+                      </c:pt>
                       <c:pt idx="6">
-                        <c:v>50</c:v>
+                        <c:v>100</c:v>
                       </c:pt>
                       <c:pt idx="7">
-                        <c:v>70</c:v>
+                        <c:v>200</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>500</c:v>
                       </c:pt>
                       <c:pt idx="9">
                         <c:v>1000</c:v>
-                      </c:pt>
-                      <c:pt idx="10">
-                        <c:v>100</c:v>
-                      </c:pt>
-                      <c:pt idx="11">
-                        <c:v>500</c:v>
-                      </c:pt>
-                      <c:pt idx="12">
-                        <c:v>200</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -693,23 +702,23 @@
                       <c:pt idx="3">
                         <c:v>302</c:v>
                       </c:pt>
+                      <c:pt idx="4">
+                        <c:v>301</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>305</c:v>
+                      </c:pt>
                       <c:pt idx="6">
-                        <c:v>301</c:v>
+                        <c:v>305</c:v>
                       </c:pt>
                       <c:pt idx="7">
-                        <c:v>305</c:v>
+                        <c:v>307</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>302</c:v>
                       </c:pt>
                       <c:pt idx="9">
                         <c:v>302</c:v>
-                      </c:pt>
-                      <c:pt idx="10">
-                        <c:v>305</c:v>
-                      </c:pt>
-                      <c:pt idx="11">
-                        <c:v>302</c:v>
-                      </c:pt>
-                      <c:pt idx="12">
-                        <c:v>307</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -750,7 +759,7 @@
                 </c:marker>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$A$5:$A$19</c15:sqref>
@@ -769,30 +778,30 @@
                       <c:pt idx="3">
                         <c:v>20</c:v>
                       </c:pt>
+                      <c:pt idx="4">
+                        <c:v>50</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>70</c:v>
+                      </c:pt>
                       <c:pt idx="6">
-                        <c:v>50</c:v>
+                        <c:v>100</c:v>
                       </c:pt>
                       <c:pt idx="7">
-                        <c:v>70</c:v>
+                        <c:v>200</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>500</c:v>
                       </c:pt>
                       <c:pt idx="9">
                         <c:v>1000</c:v>
-                      </c:pt>
-                      <c:pt idx="10">
-                        <c:v>100</c:v>
-                      </c:pt>
-                      <c:pt idx="11">
-                        <c:v>500</c:v>
-                      </c:pt>
-                      <c:pt idx="12">
-                        <c:v>200</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$C$5:$C$19</c15:sqref>
@@ -811,29 +820,29 @@
                       <c:pt idx="3">
                         <c:v>54.4</c:v>
                       </c:pt>
+                      <c:pt idx="4">
+                        <c:v>153</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>250</c:v>
+                      </c:pt>
                       <c:pt idx="6">
-                        <c:v>153</c:v>
+                        <c:v>337</c:v>
                       </c:pt>
                       <c:pt idx="7">
-                        <c:v>250</c:v>
+                        <c:v>331</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>301</c:v>
                       </c:pt>
                       <c:pt idx="9">
                         <c:v>297</c:v>
-                      </c:pt>
-                      <c:pt idx="10">
-                        <c:v>337</c:v>
-                      </c:pt>
-                      <c:pt idx="11">
-                        <c:v>301</c:v>
-                      </c:pt>
-                      <c:pt idx="12">
-                        <c:v>331</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000001-92AD-4C6D-B0E9-B25686F754B8}"/>
                   </c:ext>
@@ -868,7 +877,7 @@
                 </c:marker>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$A$5:$A$19</c15:sqref>
@@ -887,30 +896,30 @@
                       <c:pt idx="3">
                         <c:v>20</c:v>
                       </c:pt>
+                      <c:pt idx="4">
+                        <c:v>50</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>70</c:v>
+                      </c:pt>
                       <c:pt idx="6">
-                        <c:v>50</c:v>
+                        <c:v>100</c:v>
                       </c:pt>
                       <c:pt idx="7">
-                        <c:v>70</c:v>
+                        <c:v>200</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>500</c:v>
                       </c:pt>
                       <c:pt idx="9">
                         <c:v>1000</c:v>
-                      </c:pt>
-                      <c:pt idx="10">
-                        <c:v>100</c:v>
-                      </c:pt>
-                      <c:pt idx="11">
-                        <c:v>500</c:v>
-                      </c:pt>
-                      <c:pt idx="12">
-                        <c:v>200</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$D$5:$D$19</c15:sqref>
@@ -929,29 +938,29 @@
                       <c:pt idx="3">
                         <c:v>85</c:v>
                       </c:pt>
+                      <c:pt idx="4">
+                        <c:v>85</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>72</c:v>
+                      </c:pt>
                       <c:pt idx="6">
-                        <c:v>85</c:v>
+                        <c:v>47</c:v>
                       </c:pt>
                       <c:pt idx="7">
-                        <c:v>72</c:v>
+                        <c:v>15</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>5</c:v>
                       </c:pt>
                       <c:pt idx="9">
                         <c:v>2</c:v>
-                      </c:pt>
-                      <c:pt idx="10">
-                        <c:v>47</c:v>
-                      </c:pt>
-                      <c:pt idx="11">
-                        <c:v>5</c:v>
-                      </c:pt>
-                      <c:pt idx="12">
-                        <c:v>15</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000002-92AD-4C6D-B0E9-B25686F754B8}"/>
                   </c:ext>
@@ -986,7 +995,7 @@
                 </c:marker>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$A$5:$A$19</c15:sqref>
@@ -1005,30 +1014,30 @@
                       <c:pt idx="3">
                         <c:v>20</c:v>
                       </c:pt>
+                      <c:pt idx="4">
+                        <c:v>50</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>70</c:v>
+                      </c:pt>
                       <c:pt idx="6">
-                        <c:v>50</c:v>
+                        <c:v>100</c:v>
                       </c:pt>
                       <c:pt idx="7">
-                        <c:v>70</c:v>
+                        <c:v>200</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>500</c:v>
                       </c:pt>
                       <c:pt idx="9">
                         <c:v>1000</c:v>
-                      </c:pt>
-                      <c:pt idx="10">
-                        <c:v>100</c:v>
-                      </c:pt>
-                      <c:pt idx="11">
-                        <c:v>500</c:v>
-                      </c:pt>
-                      <c:pt idx="12">
-                        <c:v>200</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$E$5:$E$19</c15:sqref>
@@ -1042,7 +1051,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000003-92AD-4C6D-B0E9-B25686F754B8}"/>
                   </c:ext>
@@ -1077,7 +1086,7 @@
                 </c:marker>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$A$5:$A$19</c15:sqref>
@@ -1096,30 +1105,30 @@
                       <c:pt idx="3">
                         <c:v>20</c:v>
                       </c:pt>
+                      <c:pt idx="4">
+                        <c:v>50</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>70</c:v>
+                      </c:pt>
                       <c:pt idx="6">
-                        <c:v>50</c:v>
+                        <c:v>100</c:v>
                       </c:pt>
                       <c:pt idx="7">
-                        <c:v>70</c:v>
+                        <c:v>200</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>500</c:v>
                       </c:pt>
                       <c:pt idx="9">
                         <c:v>1000</c:v>
-                      </c:pt>
-                      <c:pt idx="10">
-                        <c:v>100</c:v>
-                      </c:pt>
-                      <c:pt idx="11">
-                        <c:v>500</c:v>
-                      </c:pt>
-                      <c:pt idx="12">
-                        <c:v>200</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$F$5:$F$19</c15:sqref>
@@ -1138,20 +1147,29 @@
                       <c:pt idx="3">
                         <c:v>134.44263297095637</c:v>
                       </c:pt>
+                      <c:pt idx="4">
+                        <c:v>125.43197340130185</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>121.28166871927192</c:v>
+                      </c:pt>
                       <c:pt idx="6">
-                        <c:v>125.43197340130185</c:v>
-                      </c:pt>
-                      <c:pt idx="10">
                         <c:v>118.6878708752859</c:v>
                       </c:pt>
-                      <c:pt idx="12">
+                      <c:pt idx="7">
                         <c:v>118.90067973980632</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>119.58328105304311</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>119.69948197857573</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000004-92AD-4C6D-B0E9-B25686F754B8}"/>
                   </c:ext>
@@ -3773,7 +3791,7 @@
   <dimension ref="A1:J37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3835,7 +3853,7 @@
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1">
-        <f t="shared" ref="F6:F19" si="0">20*LOG(B6*$F$22/C6)</f>
+        <f>20*LOG(B6*$F$22/C6)</f>
         <v>145.84053582756604</v>
       </c>
       <c r="G6" s="1">
@@ -3858,11 +3876,11 @@
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1">
-        <f t="shared" si="0"/>
+        <f>20*LOG(B7*$F$22/C7)</f>
         <v>140.40551911948623</v>
       </c>
       <c r="G7" s="1">
-        <f t="shared" ref="G7:G17" si="1">B7*$F$22/C7</f>
+        <f t="shared" ref="G7:G17" si="0">B7*$F$22/C7</f>
         <v>10477941.176470589</v>
       </c>
     </row>
@@ -3881,80 +3899,119 @@
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1">
+        <f>20*LOG(B8*$F$22/C8)</f>
+        <v>134.44263297095637</v>
+      </c>
+      <c r="G8" s="1">
         <f t="shared" si="0"/>
-        <v>134.44263297095637</v>
-      </c>
-      <c r="G8" s="1">
-        <f t="shared" si="1"/>
         <v>5273897.0588235296</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>50</v>
+      </c>
+      <c r="B9">
+        <v>301</v>
+      </c>
+      <c r="C9">
+        <v>153</v>
+      </c>
+      <c r="D9">
+        <v>85</v>
+      </c>
       <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="F9" s="1">
+        <f>20*LOG(B9*$F$22/C9)</f>
+        <v>125.43197340130185</v>
+      </c>
+      <c r="G9" s="1"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>70</v>
+      </c>
+      <c r="B10">
+        <v>305</v>
+      </c>
+      <c r="C10">
+        <v>250</v>
+      </c>
+      <c r="D10">
+        <v>72</v>
+      </c>
       <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="F10" s="1">
+        <f>20*LOG(B10*$F$22/C10)</f>
+        <v>121.28166871927192</v>
+      </c>
+      <c r="G10" s="1"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="B11">
-        <v>301</v>
+        <v>305</v>
       </c>
       <c r="C11">
-        <v>153</v>
+        <v>337</v>
       </c>
       <c r="D11">
-        <v>85</v>
+        <v>47</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1">
+        <f>20*LOG(B11*$F$22/C11)</f>
+        <v>118.6878708752859</v>
+      </c>
+      <c r="G11" s="1">
         <f t="shared" si="0"/>
-        <v>125.43197340130185</v>
-      </c>
-      <c r="G11" s="1">
-        <f t="shared" si="1"/>
-        <v>1868954.2483660132</v>
+        <v>859792.28486646886</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>70</v>
+        <v>200</v>
       </c>
       <c r="B12">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="C12">
-        <v>250</v>
+        <v>331</v>
       </c>
       <c r="D12">
-        <v>72</v>
+        <v>15</v>
       </c>
       <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
+      <c r="F12" s="1">
+        <f>20*LOG(B12*$F$22/C12)</f>
+        <v>118.90067973980632</v>
+      </c>
       <c r="G12" s="1">
-        <f t="shared" si="1"/>
-        <v>1159000</v>
+        <f t="shared" si="0"/>
+        <v>881117.82477341394</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>500</v>
+      </c>
+      <c r="B13">
+        <v>302</v>
+      </c>
+      <c r="C13">
+        <v>301</v>
+      </c>
+      <c r="D13">
+        <v>5</v>
+      </c>
       <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="F13" s="1">
+        <f>20*LOG(B13*$F$22/C13)</f>
+        <v>119.58328105304311</v>
+      </c>
+      <c r="G13" s="1"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
@@ -3970,76 +4027,37 @@
         <v>2</v>
       </c>
       <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
+      <c r="F14" s="1">
+        <f>20*LOG(B14*$F$22/C14)</f>
+        <v>119.69948197857573</v>
+      </c>
       <c r="G14" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>965993.26599326602</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>100</v>
-      </c>
-      <c r="B15">
-        <v>305</v>
-      </c>
-      <c r="C15">
-        <v>337</v>
-      </c>
-      <c r="D15">
-        <v>47</v>
-      </c>
       <c r="E15" s="1"/>
-      <c r="F15" s="1">
+      <c r="F15" s="1"/>
+      <c r="G15" s="1" t="e">
         <f t="shared" si="0"/>
-        <v>118.6878708752859</v>
-      </c>
-      <c r="G15" s="1">
-        <f t="shared" si="1"/>
-        <v>859792.28486646886</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>500</v>
-      </c>
-      <c r="B16">
-        <v>302</v>
-      </c>
-      <c r="C16">
-        <v>301</v>
-      </c>
-      <c r="D16">
-        <v>5</v>
-      </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
-      <c r="G16" s="1">
-        <f t="shared" si="1"/>
-        <v>953156.14617940201</v>
+      <c r="G16" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>200</v>
-      </c>
-      <c r="B17">
-        <v>307</v>
-      </c>
-      <c r="C17">
-        <v>331</v>
-      </c>
-      <c r="D17">
-        <v>15</v>
-      </c>
       <c r="E17" s="1"/>
-      <c r="F17" s="1">
+      <c r="F17" s="1"/>
+      <c r="G17" s="1" t="e">
         <f t="shared" si="0"/>
-        <v>118.90067973980632</v>
-      </c>
-      <c r="G17" s="1">
-        <f t="shared" si="1"/>
-        <v>881117.82477341394</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -4107,7 +4125,7 @@
         <v>240</v>
       </c>
       <c r="E26" s="1">
-        <f t="shared" ref="E26:E37" si="2">20*LOG(B26*$F$22/C26)</f>
+        <f t="shared" ref="E26:E37" si="1">20*LOG(B26*$F$22/C26)</f>
         <v>117.45186524068201</v>
       </c>
     </row>
@@ -4125,7 +4143,7 @@
         <v>260</v>
       </c>
       <c r="E27" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>145.57507201905656</v>
       </c>
     </row>
@@ -4143,67 +4161,67 @@
         <v>82</v>
       </c>
       <c r="E28" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>124.1772486135087</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E29" s="1" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E30" s="1" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E31" s="1" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E32" s="1" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="33" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E33" s="1" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="34" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E34" s="1" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="35" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E35" s="1" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="36" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E36" s="1" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="37" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E37" s="1" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A5:F19">
-    <sortCondition ref="A5:A19"/>
+  <sortState ref="A6:F17">
+    <sortCondition ref="A6:A17"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
mitad del informe del 2 y del 4
</commit_message>
<xml_diff>
--- a/Ej2/Mediciones/tc_tp2_ej2 impedancia de entrada.xlsx
+++ b/Ej2/Mediciones/tc_tp2_ej2 impedancia de entrada.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
   <si>
     <t>f(kHz)</t>
   </si>
@@ -36,9 +36,6 @@
   </si>
   <si>
     <t>fase (°)</t>
-  </si>
-  <si>
-    <t>R1(Ohm)</t>
   </si>
   <si>
     <t>|Z| dB</t>
@@ -208,31 +205,31 @@
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="1">
-                  <c:v>145.84053582756604</c:v>
+                  <c:v>126.11058523563899</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>140.40551911948623</c:v>
+                  <c:v>120.67556852755916</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>134.44263297095637</c:v>
+                  <c:v>114.71268237902932</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>125.43197340130185</c:v>
+                  <c:v>105.7020228093748</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>121.28166871927192</c:v>
+                  <c:v>101.55171812734487</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>118.6878708752859</c:v>
+                  <c:v>98.957920283358845</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>118.90067973980632</c:v>
+                  <c:v>99.170729147879243</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>119.58328105304311</c:v>
+                  <c:v>99.853330461116045</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>119.69948197857573</c:v>
+                  <c:v>99.969531386648654</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -553,16 +550,16 @@
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>124.14298906419086</c:v>
+                  <c:v>104.41303847226379</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>117.45186524068201</c:v>
+                  <c:v>97.721914648754932</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>145.57507201905656</c:v>
+                  <c:v>125.84512142712953</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>124.1772486135087</c:v>
+                  <c:v>104.44729802158163</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -1139,31 +1136,31 @@
                       <c:formatCode>0.00E+00</c:formatCode>
                       <c:ptCount val="15"/>
                       <c:pt idx="1">
-                        <c:v>145.84053582756604</c:v>
+                        <c:v>126.11058523563899</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>140.40551911948623</c:v>
+                        <c:v>120.67556852755916</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>134.44263297095637</c:v>
+                        <c:v>114.71268237902932</c:v>
                       </c:pt>
                       <c:pt idx="4">
-                        <c:v>125.43197340130185</c:v>
+                        <c:v>105.7020228093748</c:v>
                       </c:pt>
                       <c:pt idx="5">
-                        <c:v>121.28166871927192</c:v>
+                        <c:v>101.55171812734487</c:v>
                       </c:pt>
                       <c:pt idx="6">
-                        <c:v>118.6878708752859</c:v>
+                        <c:v>98.957920283358845</c:v>
                       </c:pt>
                       <c:pt idx="7">
-                        <c:v>118.90067973980632</c:v>
+                        <c:v>99.170729147879243</c:v>
                       </c:pt>
                       <c:pt idx="8">
-                        <c:v>119.58328105304311</c:v>
+                        <c:v>99.853330461116045</c:v>
                       </c:pt>
                       <c:pt idx="9">
-                        <c:v>119.69948197857573</c:v>
+                        <c:v>99.969531386648654</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -3382,16 +3379,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>352425</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3791,7 +3788,7 @@
   <dimension ref="A1:J37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="G6" sqref="G6:G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3813,14 +3810,9 @@
         <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="1">
-        <v>990000</v>
-      </c>
+      <c r="J1" s="1"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E2" s="1"/>
@@ -3828,10 +3820,10 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -3853,12 +3845,16 @@
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1">
-        <f>20*LOG(B6*$F$22/C6)</f>
-        <v>145.84053582756604</v>
+        <f>20*LOG10(B6*$F$22/C6)</f>
+        <v>126.11058523563899</v>
       </c>
       <c r="G6" s="1">
-        <f>B6*$F$22/C6</f>
-        <v>19589655.172413792</v>
+        <f>C6/$F$22</f>
+        <v>1.4795918367346939E-4</v>
+      </c>
+      <c r="I6" s="1">
+        <f>20*LOG(B6/G6)</f>
+        <v>126.11058523563899</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -3876,12 +3872,16 @@
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1">
-        <f>20*LOG(B7*$F$22/C7)</f>
-        <v>140.40551911948623</v>
+        <f t="shared" ref="F7:F14" si="0">20*LOG10(B7*$F$22/C7)</f>
+        <v>120.67556852755916</v>
       </c>
       <c r="G7" s="1">
-        <f t="shared" ref="G7:G17" si="0">B7*$F$22/C7</f>
-        <v>10477941.176470589</v>
+        <f t="shared" ref="G7:G14" si="1">C7/$F$22</f>
+        <v>2.7755102040816324E-4</v>
+      </c>
+      <c r="I7" s="1">
+        <f t="shared" ref="I7:I14" si="2">20*LOG(B7/G7)</f>
+        <v>120.67556852755916</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -3899,12 +3899,16 @@
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1">
-        <f>20*LOG(B8*$F$22/C8)</f>
-        <v>134.44263297095637</v>
+        <f t="shared" si="0"/>
+        <v>114.71268237902932</v>
       </c>
       <c r="G8" s="1">
-        <f t="shared" si="0"/>
-        <v>5273897.0588235296</v>
+        <f t="shared" si="1"/>
+        <v>5.5510204081632647E-4</v>
+      </c>
+      <c r="I8" s="1">
+        <f t="shared" si="2"/>
+        <v>114.71268237902932</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -3922,10 +3926,17 @@
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1">
-        <f>20*LOG(B9*$F$22/C9)</f>
-        <v>125.43197340130185</v>
-      </c>
-      <c r="G9" s="1"/>
+        <f t="shared" si="0"/>
+        <v>105.7020228093748</v>
+      </c>
+      <c r="G9" s="1">
+        <f t="shared" si="1"/>
+        <v>1.5612244897959184E-3</v>
+      </c>
+      <c r="I9" s="1">
+        <f t="shared" si="2"/>
+        <v>105.7020228093748</v>
+      </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -3942,10 +3953,17 @@
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1">
-        <f>20*LOG(B10*$F$22/C10)</f>
-        <v>121.28166871927192</v>
-      </c>
-      <c r="G10" s="1"/>
+        <f t="shared" si="0"/>
+        <v>101.55171812734487</v>
+      </c>
+      <c r="G10" s="1">
+        <f t="shared" si="1"/>
+        <v>2.5510204081632651E-3</v>
+      </c>
+      <c r="I10" s="1">
+        <f t="shared" si="2"/>
+        <v>101.55171812734487</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -3962,12 +3980,16 @@
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1">
-        <f>20*LOG(B11*$F$22/C11)</f>
-        <v>118.6878708752859</v>
+        <f t="shared" si="0"/>
+        <v>98.957920283358845</v>
       </c>
       <c r="G11" s="1">
-        <f t="shared" si="0"/>
-        <v>859792.28486646886</v>
+        <f t="shared" si="1"/>
+        <v>3.4387755102040815E-3</v>
+      </c>
+      <c r="I11" s="1">
+        <f t="shared" si="2"/>
+        <v>98.957920283358845</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -3985,12 +4007,16 @@
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1">
-        <f>20*LOG(B12*$F$22/C12)</f>
-        <v>118.90067973980632</v>
+        <f t="shared" si="0"/>
+        <v>99.170729147879243</v>
       </c>
       <c r="G12" s="1">
-        <f t="shared" si="0"/>
-        <v>881117.82477341394</v>
+        <f t="shared" si="1"/>
+        <v>3.3775510204081633E-3</v>
+      </c>
+      <c r="I12" s="1">
+        <f t="shared" si="2"/>
+        <v>99.170729147879243</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -4008,10 +4034,17 @@
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1">
-        <f>20*LOG(B13*$F$22/C13)</f>
-        <v>119.58328105304311</v>
-      </c>
-      <c r="G13" s="1"/>
+        <f t="shared" si="0"/>
+        <v>99.853330461116045</v>
+      </c>
+      <c r="G13" s="1">
+        <f t="shared" si="1"/>
+        <v>3.0714285714285713E-3</v>
+      </c>
+      <c r="I13" s="1">
+        <f t="shared" si="2"/>
+        <v>99.853330461116045</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
@@ -4028,37 +4061,32 @@
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1">
-        <f>20*LOG(B14*$F$22/C14)</f>
-        <v>119.69948197857573</v>
+        <f t="shared" si="0"/>
+        <v>99.969531386648654</v>
       </c>
       <c r="G14" s="1">
-        <f t="shared" si="0"/>
-        <v>965993.26599326602</v>
+        <f t="shared" si="1"/>
+        <v>3.0306122448979594E-3</v>
+      </c>
+      <c r="I14" s="1">
+        <f t="shared" si="2"/>
+        <v>99.969531386648654</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
-      <c r="G15" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="G15" s="1"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
-      <c r="G16" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="G16" s="1"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
-      <c r="G17" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="G17" s="1"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E18" s="1"/>
@@ -4070,10 +4098,10 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F22" s="1">
-        <v>950000</v>
+        <v>98000</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -4081,16 +4109,16 @@
         <v>0</v>
       </c>
       <c r="B24" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" t="s">
         <v>6</v>
-      </c>
-      <c r="C24" t="s">
-        <v>7</v>
       </c>
       <c r="D24" t="s">
         <v>3</v>
       </c>
       <c r="E24" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -4108,7 +4136,7 @@
       </c>
       <c r="E25" s="1">
         <f>20*LOG(B25*$F$22/C25)</f>
-        <v>124.14298906419086</v>
+        <v>104.41303847226379</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -4125,8 +4153,8 @@
         <v>240</v>
       </c>
       <c r="E26" s="1">
-        <f t="shared" ref="E26:E37" si="1">20*LOG(B26*$F$22/C26)</f>
-        <v>117.45186524068201</v>
+        <f t="shared" ref="E26:E37" si="3">20*LOG(B26*$F$22/C26)</f>
+        <v>97.721914648754932</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -4143,8 +4171,8 @@
         <v>260</v>
       </c>
       <c r="E27" s="1">
-        <f t="shared" si="1"/>
-        <v>145.57507201905656</v>
+        <f t="shared" si="3"/>
+        <v>125.84512142712953</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -4161,61 +4189,61 @@
         <v>82</v>
       </c>
       <c r="E28" s="1">
-        <f t="shared" si="1"/>
-        <v>124.1772486135087</v>
+        <f t="shared" si="3"/>
+        <v>104.44729802158163</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E29" s="1" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E30" s="1" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E31" s="1" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E32" s="1" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="33" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E33" s="1" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="34" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E34" s="1" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="35" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E35" s="1" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="36" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E36" s="1" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="37" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E37" s="1" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>

</xml_diff>